<commit_message>
new regression bruteForce results
</commit_message>
<xml_diff>
--- a/results/BruteForce.xlsx
+++ b/results/BruteForce.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
   <si>
     <t xml:space="preserve">3/5: For the implementation I used the ideas from https://www.cs.bgu.ac.il/~orlovm/papers/partitions.pdf to generate the set partitions efficiently!</t>
   </si>
@@ -167,10 +167,70 @@
     <t xml:space="preserve">VAL ERROR</t>
   </si>
   <si>
+    <t xml:space="preserve">Best Training Individuals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Test Individuals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 2 2 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 2 2 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 2 1 1 1 1 2 2 2 2 2 2 2 ;; 1 1 2 2 3 3 4 4 5 5 6 6 7 7 8 8 ;; 1 1 1 1 1 1 1 1 2 2 2 2 2 2 2 2 ;; 1 1 1 1 2 2 2 2 3 3 3 3 4 4 4 4 ;; 1 1 1 1 1 1 1 1 2 2 2 2 2 2 2 2 ;; 1 1 1 2 1 2 2 2 1 1 1 1 2 2 2 2 ;; 1 1 1 2 2 1 1 1 1 2 2 1 2 2 2 2 ;; 1 1 1 2 1 1 1 1 1 2 2 2 2 2 2 2 ;; 1 1 1 2 2 1 1 1 1 1 2 2 2 2 2 2 ;; 1 1 1 1 1 1 1 1 2 2 2 2 2 2 2 2 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 1 1 2 2 2 3 2 2 2 3 ;; 1 1 1 1 1 1 1 1 2 2 2 3 4 4 4 4 ;; 1 1 1 1 1 1 1 1 2 2 2 1 2 2 2 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 2 2 2 3 2 3 3 2 ;; 1 1 1 1 1 1 1 1 2 2 2 3 1 3 3 3 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 1 1 1 1 1 1 1 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 2 2 2 2 3 1 2 3 3 3 ;; 1 1 1 1 1 1 1 2 2 2 2 2 2 2 ;; 1 1 1 1 1 2 2 3 2 2 3 3 3 3 ;; 1 1 1 1 1 2 2 2 2 1 1 2 2 2 ;; 1 1 2 1 3 2 2 3 3 1 2 2 3 3 ;; 1 1 2 1 1 2 2 3 3 1 2 2 3 3 ;; 1 1 1 1 1 2 2 2 2 2 3 3 3 3 ;; 1 1 1 1 2 2 1 2 2 2 3 3 3 3 ;; 1 1 1 1 1 2 2 2 2 3 3 3 3 3 ;; 1 1 1 1 1 2 2 2 2 2 3 3 3 3 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 2 2 2 2 3 1 3 3 2 3 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;[0] ****\n</t>
+  </si>
+  <si>
     <t xml:space="preserve">TRAIN-VAL</t>
   </si>
   <si>
     <t xml:space="preserve">TEST ERROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 2 2 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 2 2 ;[1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 1 1 1 1 1 1 1 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;[1] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;[1] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;; 1 2 3 4 5 6 7 8 ;[1] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 2 2 2 2 3 1 2 3 3 3 ;; 1 1 1 1 1 1 1 2 2 2 2 2 2 2 ;; 1 1 1 1 1 2 2 3 2 2 3 3 3 3 ;; 1 1 1 1 1 2 2 2 2 1 1 2 2 2 ;; 1 1 2 1 3 2 2 3 3 1 2 2 3 3 ;; 1 1 2 1 1 2 2 3 3 1 2 2 3 3 ;; 1 1 1 1 1 2 2 2 2 2 3 3 3 3 ;; 1 1 1 1 2 2 1 2 2 2 3 3 3 3 ;; 1 1 1 1 1 2 2 2 2 3 3 3 3 3 ;; 1 1 1 1 1 2 2 2 2 2 3 3 3 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 2 2 2 2 3 1 3 3 2 3 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;[1] </t>
   </si>
   <si>
     <t xml:space="preserve">WITHOUT PRUNING</t>
@@ -403,19 +463,21 @@
   <dimension ref="B2:M54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E58" activeCellId="0" sqref="E58"/>
+      <selection pane="topLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.1632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="6" style="0" width="8.63775510204082"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.5918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.1479591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="68.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -860,7 +922,7 @@
         <v>1286.290481858</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="9" t="n">
         <v>42592</v>
       </c>
@@ -886,22 +948,34 @@
       <c r="F36" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="G36" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>48.28189</v>
+        <v>57.80229</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>247.909243125</v>
+        <v>298.8189875</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>480.69950875</v>
+        <v>499.45816875</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>253.61631875</v>
+        <v>257.339588125</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -909,41 +983,71 @@
         <v>16</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>248.34427375</v>
+        <v>250.20336875</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>417.876940625</v>
+        <v>506.033660625</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>694.44447</v>
+        <v>745.321853125</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>396.40792125</v>
+        <v>355.17583875</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="C39" s="0" t="n">
+        <v>0.63036875</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>6.68499625</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>81.23847125</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>6.47229</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>0.5683025</v>
+        <v>0.64528375</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>5.3052375</v>
+        <v>6.706185</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>81.02635375</v>
+        <v>72.31993</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>5.290275</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6.4946775</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="6" t="s">
         <v>23</v>
       </c>
@@ -953,16 +1057,22 @@
         <v>26</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>30.29945</v>
+        <v>32.77307</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>77.655293125</v>
+        <v>99.173618125</v>
       </c>
       <c r="E42" s="0" t="n">
-        <v>293.96548125</v>
+        <v>301.95774125</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>76.184513125</v>
+        <v>78.458145</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -970,31 +1080,44 @@
         <v>27</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>0.804311428571428</v>
+        <v>0.805282142857143</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>0.889969285714286</v>
+        <v>0.902631428571429</v>
       </c>
       <c r="E43" s="0" t="n">
-        <v>0.960689285714286</v>
+        <v>0.961052857142857</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>0.872181428571428</v>
-      </c>
-    </row>
+        <v>0.881771428571428</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="3" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E46" s="0" t="s">
         <v>11</v>
       </c>
       <c r="F46" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,44 +1136,80 @@
       <c r="F47" s="0" t="n">
         <v>252.60072</v>
       </c>
+      <c r="G47" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H47" s="0" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>248.34427375</v>
+        <v>248.692281875</v>
       </c>
       <c r="D48" s="0" t="n">
-        <v>486.702450625</v>
+        <v>486.704245</v>
       </c>
       <c r="E48" s="0" t="n">
-        <v>747.48596</v>
+        <v>729.04601</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>378.3230375</v>
+        <v>378.521649375</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="H48" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="C49" s="0" t="n">
+        <v>0.5366425</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>5.4100575</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>81.12135375</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>5.27375375</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="H49" s="0" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>0.5683025</v>
+        <v>0.57962375</v>
       </c>
       <c r="D50" s="0" t="n">
-        <v>5.433545</v>
+        <v>5.42545125</v>
       </c>
       <c r="E50" s="0" t="n">
-        <v>81.13725875</v>
+        <v>81.1409175</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>5.290275</v>
+        <v>5.290625</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="H50" s="0" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1074,6 +1233,12 @@
       <c r="F52" s="0" t="n">
         <v>76.184513125</v>
       </c>
+      <c r="G52" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="4" t="s">
@@ -1090,6 +1255,12 @@
       </c>
       <c r="F53" s="0" t="n">
         <v>0.876006428571428</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1100,6 +1271,24 @@
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1124,12 +1313,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1156,7 +1345,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1164,7 +1353,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1178,10 +1367,10 @@
         <v>21.26382499999</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1195,10 +1384,10 @@
         <v>21.256375</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,7 +1395,7 @@
         <v>23</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,7 +1403,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1228,10 +1417,10 @@
         <v>0.851564285714286</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
few classification results correction
</commit_message>
<xml_diff>
--- a/results/BruteForce.xlsx
+++ b/results/BruteForce.xlsx
@@ -240,70 +240,70 @@
     <t xml:space="preserve">CLASSIFICATION DATASETS</t>
   </si>
   <si>
+    <t xml:space="preserve">AUROC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test AUCPR of the best training Invidual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training AUCPR of the best test Invidual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of outputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corel5k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emotions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;[0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 2 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 2 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 2 ;; 1 1 1 1 1 2 ;; 1 1 1 1 1 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">yeast</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 1 1 1 1 1 2 2 1 3 4 3 4 5 ;; 1 1 1 1 1 1 1 1 2 1 2 2 2 1 ;; 1 1 1 1 1 1 1 1 2 3 3 3 3 1 ;; 1 1 1 1 1 1 1 1 2 3 3 1 4 1 ;; 1 1 1 1 1 1 1 1 2 1 2 2 2 2 ;; 1 1 1 1 1 1 1 1 2 2 2 2 2 1 ;; 1 1 1 1 1 1 1 2 2 3 4 2 2 5 ;; 1 1 1 1 1 1 1 1 2 2 2 2 2 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 2 2 3 2 2 1 2 2 2 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 1 2 3 2 4 4 ;; 1 1 2 3 2 4 4 ;; 1 2 3 1 2 3 4 ;; 1 1 2 2 3 3 4 ;; 1 2 3 4 5 6 7 ;; 1 1 2 2 3 3 4 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 3 1 4 3 ;; 1 2 1 1 3 3 1 ;; 1 1 2 2 1 3 2 ;; 1 1 2 2 1 1 1 ;; 1 2 1 3 2 3 1 ;; 1 2 1 2 1 1 2 ;; 1 1 1 1 2 1 2 ;; 1 1 1 2 2 1 2 ;; 1 1 1 2 2 3 3 ;; 1 2 1 1 2 3 3 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">genbase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mediamill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST</t>
+  </si>
+  <si>
     <t xml:space="preserve">AUCPR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dataset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test AUCPR of the best training Invidual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Training AUCPR of the best test Invidual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of outputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">corel5k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emotions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;[0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 2 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 2 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 2 ;; 1 1 1 1 1 2 ;; 1 1 1 1 1 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yeast</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 1 1 1 1 1 2 2 1 3 4 3 4 5 ;; 1 1 1 1 1 1 1 1 2 1 2 2 2 1 ;; 1 1 1 1 1 1 1 1 2 3 3 3 3 1 ;; 1 1 1 1 1 1 1 1 2 3 3 1 4 1 ;; 1 1 1 1 1 1 1 1 2 1 2 2 2 2 ;; 1 1 1 1 1 1 1 1 2 2 2 2 2 1 ;; 1 1 1 1 1 1 1 2 2 3 4 2 2 5 ;; 1 1 1 1 1 1 1 1 2 2 2 2 2 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 2 2 3 2 2 1 2 2 2 ;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flags</t>
-  </si>
-  <si>
-    <t xml:space="preserve">; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 1 2 3 2 4 4 ;; 1 1 2 3 2 4 4 ;; 1 2 3 1 2 3 4 ;; 1 1 2 2 3 3 4 ;; 1 2 3 4 5 6 7 ;; 1 1 2 2 3 3 4 ;[0] ****\n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">; 1 2 3 3 1 4 3 ;; 1 2 1 1 3 3 1 ;; 1 1 2 2 1 3 2 ;; 1 1 2 2 1 1 1 ;; 1 2 1 3 2 3 1 ;; 1 2 1 2 1 1 2 ;; 1 1 1 1 2 1 2 ;; 1 1 1 2 2 1 2 ;; 1 1 1 2 2 3 3 ;; 1 2 1 1 2 3 3 ;[0] ****\n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">genbase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mediamill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUROC</t>
   </si>
   <si>
     <t xml:space="preserve">Test AUROC of the best training Invidual</t>
@@ -1424,7 +1424,7 @@
   <dimension ref="B3:L58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1683,8 +1683,8 @@
     </row>
     <row r="31" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="13" t="s">
+    <row r="37" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="13" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
classification results AUPRC and AUCROC
</commit_message>
<xml_diff>
--- a/results/BruteForce.xlsx
+++ b/results/BruteForce.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="118">
   <si>
     <t xml:space="preserve">MAE ERRORS IN THIS STUDY</t>
   </si>
@@ -303,6 +303,24 @@
     <t xml:space="preserve">TEST</t>
   </si>
   <si>
+    <t xml:space="preserve">; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 2 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 2 ;; 1 1 1 1 1 2 ;; 1 1 1 1 1 2 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;; 1 2 3 4 5 6 7 8 9 10 11 12 13 14 ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 2 1 2 2 3 2 2 2 ;; 1 1 1 1 1 1 1 1 2 2 2 2 2 1 ;; 1 1 1 1 1 1 1 1 2 2 2 1 2 3 ;; 1 1 1 1 1 1 1 1 2 1 2 1 1 1 ;; 1 1 1 1 1 1 1 1 2 3 3 1 3 1 ;; 1 1 1 1 1 1 1 1 1 2 2 2 2 3 ;; 1 1 1 1 1 1 1 1 2 2 2 2 2 3 ;; 1 1 1 1 1 1 2 2 2 3 3 2 2 2 ;; 1 1 1 1 1 1 1 2 2 2 2 2 2 2 ;; 1 1 1 1 1 1 1 1 2 2 2 2 2 1 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 1 2 2 3 4 4 ;; 1 1 2 2 3 4 3 ;; 1 1 2 3 2 4 3 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 1 2 2 3 4 4 ;; 1 2 3 4 5 6 7 ;[0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 4 3 3 3 ;; 1 1 2 2 1 3 2 ;; 1 2 3 4 5 6 2 ;; 1 1 1 2 2 1 1 ;; 1 2 1 2 1 1 2 ;; 1 1 1 2 1 3 3 ;; 1 1 1 2 2 1 2 ;; 1 1 1 2 2 3 2 ;; 1 2 1 1 3 2 3 ;; 1 1 2 1 3 4 5 ;</t>
+  </si>
+  <si>
     <t xml:space="preserve">AUCPR</t>
   </si>
   <si>
@@ -310,6 +328,30 @@
   </si>
   <si>
     <t xml:space="preserve">Training AUROC of the best test Invidual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 2 1 2 2 ;; 1 1 1 2 2 2 ;; 1 1 1 2 2 2 ;; 1 1 1 2 2 2 ;; 1 1 1 2 2 2 ;; 1 1 1 2 2 2 ;; 1 1 1 2 2 2 ;; 1 1 2 1 2 2 ;; 1 1 1 2 2 2 ;; 1 1 1 2 2 2 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;; 1 1 1 1 1 1 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 2 2 3 3 1 2 3 4 4 4 5 5 ;; 1 1 1 2 2 2 3 3 3 4 4 4 5 5 ;; 1 1 1 2 2 2 3 3 3 4 4 5 4 5 ;; 1 1 1 2 2 2 3 3 3 4 4 4 5 5 ;; 1 1 1 2 2 2 3 3 3 4 4 4 5 5 ;; 1 1 1 2 3 4 2 2 3 3 4 4 5 5 ;; 1 1 1 2 2 2 3 3 3 4 4 4 5 5 ;; 1 1 1 2 2 2 3 3 3 4 4 4 5 5 ;; 1 1 1 2 2 2 3 3 3 4 4 4 5 5 ;; 1 1 1 2 2 2 3 3 3 4 4 4 5 5 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 1 1 1 1 1 1 1 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;; 1 2 3 4 5 6 7 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 ;; 1 1 1 1 1 1 1 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 1 1 2 2 2 ;; 1 1 1 2 2 2 ;; 1 1 1 2 2 2 ;; 1 1 1 2 2 2 ;; 1 1 1 2 2 2 ;; 1 1 1 2 2 2 ;; 1 1 1 2 2 2 ;; 1 1 1 2 2 2 ;; 1 1 2 1 2 2 ;; 1 1 1 2 2 2 ;[0] ****\n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; 1 2 3 1 1 4 2 2 3 3 4 4 5 5 ;; 1 1 1 2 2 2 3 3 3 4 4 4 5 5 ;; 1 1 1 2 2 2 3 3 3 4 4 4 5 5 ;; 1 2 3 1 4 2 3 4 5 5 1 2 3 4 ;; 1 1 1 2 2 3 3 4 2 3 4 4 5 5 ;; 1 1 1 2 3 2 3 2 3 4 4 4 5 5 ;; 1 1 1 2 2 2 3 3 3 4 4 4 5 5 ;; 1 1 1 2 2 2 3 3 4 4 5 3 4 5 ;; 1 1 1 2 2 2 3 3 3 4 4 4 5 5 ;; 1 1 1 2 2 2 3 3 3 4 4 4 5 5 ;[0] ****\n</t>
   </si>
   <si>
     <t xml:space="preserve">WITHOUT PRUNING</t>
@@ -340,9 +382,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -494,7 +537,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -551,7 +594,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -584,13 +639,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.4234693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="11" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="68.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1423,21 +1481,21 @@
   </sheetPr>
   <dimension ref="B3:L58"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G37" activeCellId="0" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.2397959183674"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="51.234693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.5051020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="24.7295918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.5051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.7908163265306"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.8775510204082"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1486,6 +1544,10 @@
       <c r="B12" s="0" t="s">
         <v>79</v>
       </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
       <c r="I12" s="0" t="n">
         <v>19</v>
       </c>
@@ -1498,6 +1560,10 @@
       <c r="B13" s="0" t="s">
         <v>80</v>
       </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
       <c r="I13" s="0" t="n">
         <v>374</v>
       </c>
@@ -1510,16 +1576,16 @@
       <c r="B14" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="14" t="n">
         <v>0.9870408</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="14" t="n">
         <v>0.604975816666667</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="14" t="n">
         <v>0.33253325</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="14" t="n">
         <v>0.691865066666666</v>
       </c>
       <c r="G14" s="0" t="s">
@@ -1540,16 +1606,16 @@
       <c r="B15" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="14" t="n">
         <v>0.994289</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="14" t="n">
         <v>0.414531835714286</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="14" t="n">
         <v>0.302904028571428</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="14" t="n">
         <v>0.555385614285714</v>
       </c>
       <c r="G15" s="0" t="s">
@@ -1570,16 +1636,16 @@
       <c r="B16" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="14" t="n">
         <v>0.851295214285714</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="14" t="n">
         <v>0.685729128571429</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="14" t="n">
         <v>0.555908514285714</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="14" t="n">
         <v>0.791426157142857</v>
       </c>
       <c r="G16" s="0" t="s">
@@ -1600,6 +1666,10 @@
       <c r="B17" s="0" t="s">
         <v>90</v>
       </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
       <c r="I17" s="0" t="n">
         <v>27</v>
       </c>
@@ -1612,6 +1682,10 @@
       <c r="B18" s="0" t="s">
         <v>91</v>
       </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
       <c r="I18" s="0" t="n">
         <v>101</v>
       </c>
@@ -1620,20 +1694,38 @@
         <v>2.53530120045646E+030</v>
       </c>
     </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+    </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="15" t="s">
         <v>77</v>
       </c>
       <c r="G22" s="4" t="s">
@@ -1650,59 +1742,185 @@
       <c r="B23" s="0" t="s">
         <v>79</v>
       </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
         <v>80</v>
       </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
         <v>81</v>
       </c>
+      <c r="C25" s="14" t="n">
+        <v>0.988858</v>
+      </c>
+      <c r="D25" s="14" t="n">
+        <v>0.604858733333333</v>
+      </c>
+      <c r="E25" s="14" t="n">
+        <v>0.337348183333333</v>
+      </c>
+      <c r="F25" s="14" t="n">
+        <v>0.697641533333333</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="C26" s="14" t="n">
+        <v>0.9944429</v>
+      </c>
+      <c r="D26" s="14" t="n">
+        <v>0.420568057142857</v>
+      </c>
+      <c r="E26" s="14" t="n">
+        <v>0.308850907142857</v>
+      </c>
+      <c r="F26" s="14" t="n">
+        <v>0.560555621428571</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
         <v>87</v>
       </c>
+      <c r="C27" s="14" t="n">
+        <v>0.863012357142857</v>
+      </c>
+      <c r="D27" s="14" t="n">
+        <v>0.689682228571429</v>
+      </c>
+      <c r="E27" s="14" t="n">
+        <v>0.597549242857143</v>
+      </c>
+      <c r="F27" s="14" t="n">
+        <v>0.811110357142857</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
         <v>90</v>
       </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="31" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+    </row>
+    <row r="32" s="16" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+    </row>
     <row r="37" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="13" t="s">
-        <v>93</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>95</v>
+      <c r="E40" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>49</v>
@@ -1719,52 +1937,140 @@
       <c r="B41" s="0" t="s">
         <v>79</v>
       </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
         <v>80</v>
       </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
         <v>81</v>
       </c>
+      <c r="C43" s="14" t="n">
+        <v>0.338965466666667</v>
+      </c>
+      <c r="D43" s="14" t="n">
+        <v>0.311827216666667</v>
+      </c>
+      <c r="E43" s="14" t="n">
+        <v>0.311827216666667</v>
+      </c>
+      <c r="F43" s="14" t="n">
+        <v>0.311421883333333</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="C44" s="14" t="n">
+        <v>0.38217515</v>
+      </c>
+      <c r="D44" s="14" t="n">
+        <v>0.302689157142857</v>
+      </c>
+      <c r="E44" s="14" t="n">
+        <v>0.302689157142857</v>
+      </c>
+      <c r="F44" s="14" t="n">
+        <v>0.302648871428571</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="H44" s="0" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
         <v>87</v>
       </c>
+      <c r="C45" s="14" t="n">
+        <v>0.7887036</v>
+      </c>
+      <c r="D45" s="14" t="n">
+        <v>0.485360485714286</v>
+      </c>
+      <c r="E45" s="14" t="n">
+        <v>0.485360485714286</v>
+      </c>
+      <c r="F45" s="14" t="n">
+        <v>0.484558685714286</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="H45" s="0" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="0" t="s">
         <v>90</v>
       </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
         <v>91</v>
       </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="E51" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>95</v>
+      <c r="E51" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="F51" s="15" t="s">
+        <v>101</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>49</v>
@@ -1780,36 +2086,106 @@
       <c r="B52" s="0" t="s">
         <v>79</v>
       </c>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
         <v>80</v>
       </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
         <v>81</v>
       </c>
+      <c r="C54" s="14" t="n">
+        <v>0.338960066666667</v>
+      </c>
+      <c r="D54" s="14" t="n">
+        <v>0.311827216666667</v>
+      </c>
+      <c r="E54" s="14" t="n">
+        <v>0.311827216666667</v>
+      </c>
+      <c r="F54" s="14" t="n">
+        <v>0.311416183333333</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="0" t="s">
         <v>84</v>
       </c>
+      <c r="C55" s="14" t="n">
+        <v>0.382174657142857</v>
+      </c>
+      <c r="D55" s="14" t="n">
+        <v>0.302689157142857</v>
+      </c>
+      <c r="E55" s="14" t="n">
+        <v>0.302689157142857</v>
+      </c>
+      <c r="F55" s="14" t="n">
+        <v>0.302648435714286</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="0" t="s">
         <v>87</v>
       </c>
+      <c r="C56" s="14" t="n">
+        <v>0.788672</v>
+      </c>
+      <c r="D56" s="14" t="n">
+        <v>0.485360485714286</v>
+      </c>
+      <c r="E56" s="14" t="n">
+        <v>0.485360485714286</v>
+      </c>
+      <c r="F56" s="14" t="n">
+        <v>0.4845451</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="0" t="s">
         <v>90</v>
       </c>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
         <v>91</v>
       </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1834,10 +2210,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,23 +2239,23 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="18" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="18" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="0" t="n">
@@ -1886,10 +2265,10 @@
         <v>21.26382499999</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,10 +2282,10 @@
         <v>21.256375</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1914,7 +2293,7 @@
         <v>24</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1922,11 +2301,11 @@
         <v>27</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="18" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="0" t="n">
@@ -1936,10 +2315,10 @@
         <v>0.851564285714286</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new BruteForce Results (validation partitioing in test)
</commit_message>
<xml_diff>
--- a/results/BruteForce.xlsx
+++ b/results/BruteForce.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="154">
   <si>
     <t xml:space="preserve">Experiments with 10 FCV: train, validation and test sets.</t>
   </si>
@@ -298,6 +298,9 @@
     <t xml:space="preserve">TEST</t>
   </si>
   <si>
+    <t xml:space="preserve">Test (best Validation-partitioning)</t>
+  </si>
+  <si>
     <t xml:space="preserve">; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 ;; 1 2 3 4 5 6 </t>
   </si>
   <si>
@@ -347,6 +350,15 @@
   </si>
   <si>
     <t xml:space="preserve">; 1 2 3 4 3 3 3 ;; 1 1 2 2 1 3 2 ;; 1 2 3 4 5 6 2 ;; 1 1 1 2 2 1 1 ;; 1 2 1 2 1 1 2 ;; 1 1 1 2 1 3 3 ;; 1 1 1 2 2 1 2 ;; 1 1 1 2 2 3 2 ;; 1 2 1 1 3 2 3 ;; 1 1 2 1 3 4 5 ;[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RunTime BruteForce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training (find a solution with the validation set)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test (time to classify the test using trainvalid)</t>
   </si>
   <si>
     <t xml:space="preserve">RESULTS USED IN THE BENELEARN ABSTRACT.  TRAINING VS. TEST</t>
@@ -741,19 +753,22 @@
   </sheetPr>
   <dimension ref="B2:H65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.0765306122449"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1820,23 +1835,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:L58"/>
+  <dimension ref="B3:M65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H49" activeCellId="0" sqref="H49"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G69" activeCellId="0" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="48.8673469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.9642857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.765306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="48.3265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1859,25 +1875,26 @@
       <c r="D11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1889,11 +1906,12 @@
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-      <c r="I12" s="0" t="n">
+      <c r="G12" s="10"/>
+      <c r="J12" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="K12" s="0" t="n">
-        <f aca="false">2^(Classification!I12)</f>
+      <c r="L12" s="0" t="n">
+        <f aca="false">2^(Classification!J12)</f>
         <v>524288</v>
       </c>
     </row>
@@ -1905,11 +1923,12 @@
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
-      <c r="I13" s="0" t="n">
+      <c r="G13" s="10"/>
+      <c r="J13" s="0" t="n">
         <v>374</v>
       </c>
-      <c r="K13" s="0" t="n">
-        <f aca="false">2^(Classification!I13)</f>
+      <c r="L13" s="0" t="n">
+        <f aca="false">2^(Classification!J13)</f>
         <v>3.84785216761665E+112</v>
       </c>
     </row>
@@ -1923,23 +1942,23 @@
       <c r="D14" s="10" t="n">
         <v>0.77435105</v>
       </c>
-      <c r="E14" s="10" t="n">
+      <c r="F14" s="10" t="n">
         <v>0.48236175</v>
       </c>
-      <c r="F14" s="10" t="n">
+      <c r="G14" s="10" t="n">
         <v>0.830021083333333</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="I14" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="J14" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="K14" s="0" t="n">
-        <f aca="false">2^(Classification!I14)</f>
+      <c r="L14" s="0" t="n">
+        <f aca="false">2^(Classification!J14)</f>
         <v>64</v>
       </c>
     </row>
@@ -1953,23 +1972,23 @@
       <c r="D15" s="10" t="n">
         <v>0.634399492857143</v>
       </c>
-      <c r="E15" s="10" t="n">
+      <c r="F15" s="10" t="n">
         <v>0.491676185714286</v>
       </c>
-      <c r="F15" s="10" t="n">
+      <c r="G15" s="10" t="n">
         <v>0.720757185714286</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="H15" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="I15" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="J15" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="K15" s="0" t="n">
-        <f aca="false">2^(Classification!I15)</f>
+      <c r="L15" s="0" t="n">
+        <f aca="false">2^(Classification!J15)</f>
         <v>16384</v>
       </c>
     </row>
@@ -1983,23 +2002,23 @@
       <c r="D16" s="10" t="n">
         <v>0.728722071428571</v>
       </c>
-      <c r="E16" s="10" t="n">
+      <c r="F16" s="10" t="n">
         <v>0.6592636</v>
       </c>
-      <c r="F16" s="10" t="n">
+      <c r="G16" s="10" t="n">
         <v>0.719985385714286</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="H16" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="I16" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="I16" s="0" t="n">
+      <c r="J16" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="K16" s="0" t="n">
-        <f aca="false">2^(Classification!I16)</f>
+      <c r="L16" s="0" t="n">
+        <f aca="false">2^(Classification!J16)</f>
         <v>128</v>
       </c>
     </row>
@@ -2011,11 +2030,12 @@
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
-      <c r="I17" s="0" t="n">
+      <c r="G17" s="10"/>
+      <c r="J17" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="K17" s="0" t="n">
-        <f aca="false">2^(Classification!I17)</f>
+      <c r="L17" s="0" t="n">
+        <f aca="false">2^(Classification!J17)</f>
         <v>134217728</v>
       </c>
     </row>
@@ -2027,11 +2047,12 @@
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
-      <c r="I18" s="0" t="n">
+      <c r="G18" s="10"/>
+      <c r="J18" s="0" t="n">
         <v>101</v>
       </c>
-      <c r="K18" s="0" t="n">
-        <f aca="false">2^(Classification!I18)</f>
+      <c r="L18" s="0" t="n">
+        <f aca="false">2^(Classification!J18)</f>
         <v>2.53530120045646E+030</v>
       </c>
     </row>
@@ -2040,18 +2061,21 @@
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
@@ -2064,20 +2088,23 @@
         <v>90</v>
       </c>
       <c r="E22" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="G22" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
@@ -2087,6 +2114,7 @@
       <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
@@ -2096,6 +2124,7 @@
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
@@ -2107,17 +2136,20 @@
       <c r="D25" s="10" t="n">
         <v>0.774763866666667</v>
       </c>
-      <c r="E25" s="10" t="n">
+      <c r="E25" s="0" t="n">
+        <v>0.772435283333333</v>
+      </c>
+      <c r="F25" s="10" t="n">
         <v>0.483692666666667</v>
       </c>
-      <c r="F25" s="10" t="n">
+      <c r="G25" s="10" t="n">
         <v>0.836423566666666</v>
-      </c>
-      <c r="G25" s="0" t="s">
-        <v>91</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>92</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2130,17 +2162,20 @@
       <c r="D26" s="10" t="n">
         <v>0.635671957142857</v>
       </c>
-      <c r="E26" s="10" t="n">
+      <c r="E26" s="0" t="n">
+        <v>0.589142714285714</v>
+      </c>
+      <c r="F26" s="10" t="n">
         <v>0.504111571428571</v>
       </c>
-      <c r="F26" s="10" t="n">
+      <c r="G26" s="10" t="n">
         <v>0.739800671428571</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>93</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>94</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2153,17 +2188,20 @@
       <c r="D27" s="10" t="n">
         <v>0.724845742857143</v>
       </c>
-      <c r="E27" s="10" t="n">
+      <c r="E27" s="0" t="n">
+        <v>0.637816714285714</v>
+      </c>
+      <c r="F27" s="10" t="n">
         <v>0.6704462</v>
       </c>
-      <c r="F27" s="10" t="n">
+      <c r="G27" s="10" t="n">
         <v>0.729182757142857</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>95</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>96</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2174,6 +2212,7 @@
       <c r="D28" s="10"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
@@ -2183,69 +2222,80 @@
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
     </row>
     <row r="31" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
     </row>
     <row r="37" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="0" t="s">
@@ -2257,22 +2307,23 @@
       <c r="D40" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E40" s="11" t="s">
-        <v>98</v>
-      </c>
+      <c r="E40" s="11"/>
       <c r="F40" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="G40" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H40" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="I40" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I40" s="5"/>
       <c r="J40" s="5"/>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
@@ -2282,6 +2333,7 @@
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
@@ -2291,6 +2343,7 @@
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
@@ -2302,17 +2355,18 @@
       <c r="D43" s="10" t="n">
         <v>0.604975816666667</v>
       </c>
-      <c r="E43" s="10" t="n">
+      <c r="E43" s="10"/>
+      <c r="F43" s="10" t="n">
         <v>0.33253325</v>
       </c>
-      <c r="F43" s="10" t="n">
+      <c r="G43" s="10" t="n">
         <v>0.691865066666666</v>
       </c>
-      <c r="G43" s="0" t="s">
+      <c r="H43" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="H43" s="0" t="s">
-        <v>100</v>
+      <c r="I43" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2325,17 +2379,18 @@
       <c r="D44" s="10" t="n">
         <v>0.414531835714286</v>
       </c>
-      <c r="E44" s="10" t="n">
+      <c r="E44" s="10"/>
+      <c r="F44" s="10" t="n">
         <v>0.302904028571428</v>
       </c>
-      <c r="F44" s="10" t="n">
+      <c r="G44" s="10" t="n">
         <v>0.555385614285714</v>
       </c>
-      <c r="G44" s="0" t="s">
+      <c r="H44" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="H44" s="0" t="s">
-        <v>101</v>
+      <c r="I44" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2348,17 +2403,18 @@
       <c r="D45" s="10" t="n">
         <v>0.685729128571429</v>
       </c>
-      <c r="E45" s="10" t="n">
+      <c r="E45" s="10"/>
+      <c r="F45" s="10" t="n">
         <v>0.555908514285714</v>
       </c>
-      <c r="F45" s="10" t="n">
+      <c r="G45" s="10" t="n">
         <v>0.791426157142857</v>
-      </c>
-      <c r="G45" s="0" t="s">
-        <v>102</v>
       </c>
       <c r="H45" s="0" t="s">
         <v>103</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2369,6 +2425,7 @@
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="0" t="s">
@@ -2378,24 +2435,28 @@
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
       <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="0" t="s">
@@ -2408,20 +2469,23 @@
         <v>90</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F51" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="G51" s="5" t="s">
+      <c r="G51" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H51" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H51" s="5" t="s">
+      <c r="I51" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I51" s="5"/>
       <c r="J51" s="5"/>
       <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="0" t="s">
@@ -2431,6 +2495,7 @@
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="0" t="s">
@@ -2440,6 +2505,7 @@
       <c r="D53" s="10"/>
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="0" t="s">
@@ -2451,17 +2517,20 @@
       <c r="D54" s="10" t="n">
         <v>0.604858733333333</v>
       </c>
-      <c r="E54" s="10" t="n">
+      <c r="E54" s="0" t="n">
+        <v>0.595064583333333</v>
+      </c>
+      <c r="F54" s="10" t="n">
         <v>0.337348183333333</v>
       </c>
-      <c r="F54" s="10" t="n">
+      <c r="G54" s="10" t="n">
         <v>0.697641533333333</v>
       </c>
-      <c r="G54" s="0" t="s">
+      <c r="H54" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="H54" s="0" t="s">
-        <v>104</v>
+      <c r="I54" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2474,17 +2543,20 @@
       <c r="D55" s="10" t="n">
         <v>0.420568057142857</v>
       </c>
-      <c r="E55" s="10" t="n">
+      <c r="E55" s="0" t="n">
+        <v>0.400292657142857</v>
+      </c>
+      <c r="F55" s="10" t="n">
         <v>0.308850907142857</v>
       </c>
-      <c r="F55" s="10" t="n">
+      <c r="G55" s="10" t="n">
         <v>0.560555621428571</v>
       </c>
-      <c r="G55" s="0" t="s">
+      <c r="H55" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="H55" s="0" t="s">
-        <v>105</v>
+      <c r="I55" s="0" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2497,17 +2569,20 @@
       <c r="D56" s="10" t="n">
         <v>0.689682228571429</v>
       </c>
-      <c r="E56" s="10" t="n">
+      <c r="E56" s="0" t="n">
+        <v>0.617537485714286</v>
+      </c>
+      <c r="F56" s="10" t="n">
         <v>0.597549242857143</v>
       </c>
-      <c r="F56" s="10" t="n">
+      <c r="G56" s="10" t="n">
         <v>0.811110357142857</v>
-      </c>
-      <c r="G56" s="0" t="s">
-        <v>106</v>
       </c>
       <c r="H56" s="0" t="s">
         <v>107</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2518,6 +2593,7 @@
       <c r="D57" s="10"/>
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="0" t="s">
@@ -2527,6 +2603,52 @@
       <c r="D58" s="10"/>
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E62" s="5"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C63" s="0" t="n">
+        <v>5.3604844735</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>0.1855323496</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" s="0" t="n">
+        <v>14307.0187818438</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>4.2036086475</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" s="0" t="n">
+        <v>1.9101926333</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>0.0455890399</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2547,48 +2669,51 @@
   <dimension ref="B3:N36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="14" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="15" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>75</v>
@@ -2597,7 +2722,7 @@
         <v>76</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="M15" s="0" t="s">
         <v>5</v>
@@ -2617,10 +2742,10 @@
         <v>437.437418749999</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H16" s="16" t="n">
         <v>10480142147</v>
@@ -2649,10 +2774,10 @@
         <v>532.88014375</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="H17" s="16" t="n">
         <v>10480142147</v>
@@ -2681,10 +2806,10 @@
         <v>21.1001875</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H18" s="0" t="n">
         <v>4140</v>
@@ -2713,10 +2838,10 @@
         <v>21.09225</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>4140</v>
@@ -2745,10 +2870,10 @@
         <v>151.66005</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H20" s="16" t="n">
         <v>10480142147</v>
@@ -2771,10 +2896,10 @@
         <v>208.48348125</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H21" s="16" t="n">
         <v>10480142147</v>
@@ -2803,10 +2928,10 @@
         <v>0.776328571428571</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="H22" s="16" t="n">
         <v>190899322</v>
@@ -2826,38 +2951,38 @@
     </row>
     <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="14" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="18" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>75</v>
@@ -2866,7 +2991,7 @@
         <v>76</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2880,10 +3005,10 @@
         <v>360.02581875</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="H30" s="16" t="n">
         <v>10480142147</v>
@@ -2906,10 +3031,10 @@
         <v>728.3298125</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="H31" s="16" t="n">
         <v>10480142147</v>
@@ -2926,10 +3051,10 @@
         <v>15</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
@@ -2945,10 +3070,10 @@
         <v>21.0327875</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="J33" s="17"/>
     </row>
@@ -2957,7 +3082,7 @@
         <v>20</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H34" s="16"/>
     </row>
@@ -2966,7 +3091,7 @@
         <v>21</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H35" s="16"/>
     </row>
@@ -2981,10 +3106,10 @@
         <v>0.9033</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H36" s="16" t="n">
         <v>190899322</v>
@@ -3019,29 +3144,32 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3049,7 +3177,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3057,7 +3185,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3071,10 +3199,10 @@
         <v>21.26382499999</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3088,10 +3216,10 @@
         <v>21.256375</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3099,7 +3227,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3107,7 +3235,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3121,10 +3249,10 @@
         <v>0.851564285714286</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>